<commit_message>
Add blood and urine SOCs to all years
</commit_message>
<xml_diff>
--- a/metadata/SSD-NHANES-2009-2010-100.xlsx
+++ b/metadata/SSD-NHANES-2009-2010-100.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/henrique/git/nhanes-hadatac/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE9DA68-53FA-5949-9394-C9AA772D0D80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48952CB-9857-9945-B0FB-65CDCA26AA4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21540" yWindow="-18500" windowWidth="27640" windowHeight="16440" activeTab="1" xr2:uid="{99F202CB-6519-5442-830D-344A4E1B0030}"/>
+    <workbookView xWindow="-21540" yWindow="-18500" windowWidth="27640" windowHeight="16440" xr2:uid="{99F202CB-6519-5442-830D-344A4E1B0030}"/>
   </bookViews>
   <sheets>
     <sheet name="SSD" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="55">
   <si>
     <t>sheet</t>
   </si>
@@ -182,6 +182,24 @@
   </si>
   <si>
     <t>nhanes-kb:SOC-NHANES-2009-2010-HH_REF_PERSON</t>
+  </si>
+  <si>
+    <t>??blood</t>
+  </si>
+  <si>
+    <t>Blood Sample</t>
+  </si>
+  <si>
+    <t>??urine</t>
+  </si>
+  <si>
+    <t>Urine Sample</t>
+  </si>
+  <si>
+    <t>nhanes-kb:SOC-NHANES-2009-2010-BLOOD</t>
+  </si>
+  <si>
+    <t>nhanes-kb:SOC-NHANES-2009-2010-URINE</t>
   </si>
 </sst>
 </file>
@@ -533,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48B088F3-3515-904B-9B51-EE2323ADDBE3}">
-  <dimension ref="A1:P9"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -759,6 +777,40 @@
         <v>47</v>
       </c>
     </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" t="s">
+        <v>50</v>
+      </c>
+      <c r="I10" t="s">
+        <v>40</v>
+      </c>
+      <c r="J10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" t="s">
+        <v>52</v>
+      </c>
+      <c r="I11" t="s">
+        <v>40</v>
+      </c>
+      <c r="J11" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -768,7 +820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E011250-3505-F946-B4F1-171B9963C1A6}">
   <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>